<commit_message>
Data toevoegen aan einde Excel bestand
</commit_message>
<xml_diff>
--- a/koersen.xlsx
+++ b/koersen.xlsx
@@ -1,352 +1,356 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16095" xWindow="240" yWindow="15"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="106">
   <si>
     <t>BEL 20</t>
   </si>
   <si>
-    <t>3.862,26</t>
-  </si>
-  <si>
-    <t>3.895,33</t>
-  </si>
-  <si>
-    <t>3.853,04</t>
-  </si>
-  <si>
-    <t>3.894,62</t>
-  </si>
-  <si>
-    <t>18:05</t>
+    <t>3.863,68</t>
+  </si>
+  <si>
+    <t>3.885,35</t>
+  </si>
+  <si>
+    <t>3.862,40</t>
+  </si>
+  <si>
+    <t>3.884,33</t>
+  </si>
+  <si>
+    <t>2018-08-08 18:00:00</t>
   </si>
   <si>
     <t>AB InBev</t>
   </si>
   <si>
-    <t>85,810</t>
-  </si>
-  <si>
-    <t>86,905</t>
-  </si>
-  <si>
-    <t>85,300</t>
-  </si>
-  <si>
-    <t>86,570</t>
-  </si>
-  <si>
-    <t>17:29</t>
+    <t>85,870</t>
+  </si>
+  <si>
+    <t>87,150</t>
+  </si>
+  <si>
+    <t>85,820</t>
+  </si>
+  <si>
+    <t>87,070</t>
+  </si>
+  <si>
+    <t>2018-08-08 17:00:00</t>
   </si>
   <si>
     <t>Ackermans &amp; v.H</t>
   </si>
   <si>
-    <t>154,600</t>
-  </si>
-  <si>
-    <t>155,900</t>
-  </si>
-  <si>
-    <t>154,300</t>
+    <t>156,500</t>
+  </si>
+  <si>
+    <t>157,200</t>
+  </si>
+  <si>
+    <t>156,200</t>
+  </si>
+  <si>
+    <t>156,800</t>
   </si>
   <si>
     <t>Ageas</t>
   </si>
   <si>
-    <t>45,500</t>
-  </si>
-  <si>
-    <t>45,860</t>
-  </si>
-  <si>
-    <t>45,150</t>
-  </si>
-  <si>
-    <t>45,900</t>
+    <t>45,510</t>
+  </si>
+  <si>
+    <t>45,530</t>
+  </si>
+  <si>
+    <t>44,070</t>
+  </si>
+  <si>
+    <t>45,230</t>
   </si>
   <si>
     <t>Aperam</t>
   </si>
   <si>
-    <t>40,290</t>
-  </si>
-  <si>
-    <t>40,390</t>
-  </si>
-  <si>
-    <t>39,800</t>
-  </si>
-  <si>
-    <t>40,690</t>
+    <t>41,180</t>
+  </si>
+  <si>
+    <t>41,330</t>
+  </si>
+  <si>
+    <t>40,630</t>
   </si>
   <si>
     <t>arGEN-X</t>
   </si>
   <si>
-    <t>79,900</t>
-  </si>
-  <si>
-    <t>80,200</t>
-  </si>
-  <si>
-    <t>77,300</t>
-  </si>
-  <si>
-    <t>79,100</t>
-  </si>
-  <si>
-    <t>17:35</t>
+    <t>78,800</t>
+  </si>
+  <si>
+    <t>79,000</t>
+  </si>
+  <si>
+    <t>77,500</t>
+  </si>
+  <si>
+    <t>78,400</t>
   </si>
   <si>
     <t>bpost</t>
   </si>
   <si>
-    <t>13,060</t>
-  </si>
-  <si>
-    <t>13,380</t>
-  </si>
-  <si>
-    <t>13,050</t>
-  </si>
-  <si>
-    <t>13,180</t>
+    <t>13,450</t>
+  </si>
+  <si>
+    <t>13,480</t>
+  </si>
+  <si>
+    <t>12,970</t>
+  </si>
+  <si>
+    <t>13,160</t>
   </si>
   <si>
     <t>Cofinimmo</t>
   </si>
   <si>
-    <t>112,000</t>
-  </si>
-  <si>
-    <t>111,600</t>
-  </si>
-  <si>
-    <t>111,700</t>
+    <t>111,400</t>
+  </si>
+  <si>
+    <t>111,900</t>
+  </si>
+  <si>
+    <t>111,000</t>
+  </si>
+  <si>
+    <t>111,800</t>
   </si>
   <si>
     <t>Colruyt</t>
   </si>
   <si>
-    <t>51,200</t>
+    <t>51,180</t>
+  </si>
+  <si>
+    <t>51,500</t>
+  </si>
+  <si>
+    <t>50,900</t>
   </si>
   <si>
     <t>51,400</t>
   </si>
   <si>
-    <t>50,860</t>
-  </si>
-  <si>
-    <t>51,300</t>
-  </si>
-  <si>
-    <t>17:28</t>
-  </si>
-  <si>
     <t>Engie</t>
   </si>
   <si>
-    <t>13,425</t>
-  </si>
-  <si>
-    <t>13,580</t>
-  </si>
-  <si>
-    <t>13,395</t>
-  </si>
-  <si>
-    <t>13,555</t>
+    <t>13,340</t>
+  </si>
+  <si>
+    <t>13,495</t>
+  </si>
+  <si>
+    <t>13,275</t>
+  </si>
+  <si>
+    <t>13,530</t>
   </si>
   <si>
     <t>Galapagos</t>
   </si>
   <si>
-    <t>92,400</t>
-  </si>
-  <si>
-    <t>94,440</t>
+    <t>96,940</t>
+  </si>
+  <si>
+    <t>98,480</t>
+  </si>
+  <si>
+    <t>95,700</t>
+  </si>
+  <si>
+    <t>97,300</t>
+  </si>
+  <si>
+    <t>GBL</t>
+  </si>
+  <si>
+    <t>89,960</t>
+  </si>
+  <si>
+    <t>90,360</t>
+  </si>
+  <si>
+    <t>89,860</t>
   </si>
   <si>
     <t>90,060</t>
   </si>
   <si>
-    <t>94,220</t>
-  </si>
-  <si>
-    <t>GBL</t>
-  </si>
-  <si>
-    <t>89,260</t>
-  </si>
-  <si>
-    <t>90,760</t>
-  </si>
-  <si>
-    <t>89,010</t>
-  </si>
-  <si>
-    <t>90,540</t>
-  </si>
-  <si>
     <t>ING</t>
   </si>
   <si>
-    <t>12,854</t>
-  </si>
-  <si>
-    <t>13,280</t>
-  </si>
-  <si>
-    <t>12,678</t>
-  </si>
-  <si>
-    <t>12,992</t>
+    <t>12,666</t>
+  </si>
+  <si>
+    <t>12,702</t>
+  </si>
+  <si>
+    <t>12,600</t>
+  </si>
+  <si>
+    <t>12,662</t>
   </si>
   <si>
     <t>KBC Groep</t>
   </si>
   <si>
-    <t>64,520</t>
-  </si>
-  <si>
-    <t>65,140</t>
-  </si>
-  <si>
-    <t>63,800</t>
-  </si>
-  <si>
-    <t>65,020</t>
+    <t>64,100</t>
+  </si>
+  <si>
+    <t>64,660</t>
+  </si>
+  <si>
+    <t>63,980</t>
+  </si>
+  <si>
+    <t>64,560</t>
   </si>
   <si>
     <t>Ontex</t>
   </si>
   <si>
-    <t>25,820</t>
-  </si>
-  <si>
-    <t>26,060</t>
-  </si>
-  <si>
-    <t>26,000</t>
+    <t>25,700</t>
+  </si>
+  <si>
+    <t>25,900</t>
+  </si>
+  <si>
+    <t>25,640</t>
+  </si>
+  <si>
+    <t>25,780</t>
   </si>
   <si>
     <t>Proximus</t>
   </si>
   <si>
-    <t>20,820</t>
-  </si>
-  <si>
-    <t>20,920</t>
-  </si>
-  <si>
-    <t>20,650</t>
-  </si>
-  <si>
-    <t>20,940</t>
+    <t>21,180</t>
+  </si>
+  <si>
+    <t>21,440</t>
+  </si>
+  <si>
+    <t>21,130</t>
+  </si>
+  <si>
+    <t>21,350</t>
   </si>
   <si>
     <t>Sofina</t>
   </si>
   <si>
-    <t>158,000</t>
-  </si>
-  <si>
-    <t>155,200</t>
-  </si>
-  <si>
-    <t>156,400</t>
-  </si>
-  <si>
-    <t>17:37</t>
+    <t>162,800</t>
+  </si>
+  <si>
+    <t>163,400</t>
+  </si>
+  <si>
+    <t>161,800</t>
+  </si>
+  <si>
+    <t>162,400</t>
   </si>
   <si>
     <t>Solvay</t>
   </si>
   <si>
-    <t>114,300</t>
-  </si>
-  <si>
-    <t>116,000</t>
-  </si>
-  <si>
-    <t>113,900</t>
-  </si>
-  <si>
-    <t>116,700</t>
+    <t>115,100</t>
+  </si>
+  <si>
+    <t>115,850</t>
+  </si>
+  <si>
+    <t>114,500</t>
+  </si>
+  <si>
+    <t>114,900</t>
   </si>
   <si>
     <t>Telenet  Group</t>
   </si>
   <si>
-    <t>44,020</t>
-  </si>
-  <si>
-    <t>44,060</t>
-  </si>
-  <si>
-    <t>42,120</t>
-  </si>
-  <si>
-    <t>43,880</t>
+    <t>44,560</t>
+  </si>
+  <si>
+    <t>44,960</t>
+  </si>
+  <si>
+    <t>44,270</t>
+  </si>
+  <si>
+    <t>45,000</t>
   </si>
   <si>
     <t>UCB</t>
   </si>
   <si>
-    <t>74,280</t>
-  </si>
-  <si>
-    <t>74,380</t>
-  </si>
-  <si>
-    <t>73,680</t>
-  </si>
-  <si>
-    <t>74,180</t>
+    <t>75,740</t>
+  </si>
+  <si>
+    <t>76,280</t>
+  </si>
+  <si>
+    <t>75,520</t>
+  </si>
+  <si>
+    <t>75,940</t>
   </si>
   <si>
     <t>Umicore</t>
   </si>
   <si>
-    <t>50,900</t>
-  </si>
-  <si>
-    <t>50,380</t>
-  </si>
-  <si>
-    <t>51,100</t>
+    <t>49,440</t>
+  </si>
+  <si>
+    <t>50,780</t>
+  </si>
+  <si>
+    <t>49,340</t>
+  </si>
+  <si>
+    <t>50,700</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -362,16 +366,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -450,6 +453,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -484,6 +488,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -659,12 +664,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -720,7 +731,7 @@
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -728,19 +739,19 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
@@ -748,19 +759,19 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
         <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -783,24 +794,24 @@
         <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -808,10 +819,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
         <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
@@ -843,24 +854,24 @@
         <v>45</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
         <v>47</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>48</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>49</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>50</v>
-      </c>
-      <c r="E10" t="s">
-        <v>51</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
@@ -868,19 +879,19 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
         <v>52</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>53</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>54</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>55</v>
-      </c>
-      <c r="E11" t="s">
-        <v>56</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
@@ -888,19 +899,19 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
         <v>57</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>58</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>59</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>60</v>
-      </c>
-      <c r="E12" t="s">
-        <v>61</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
@@ -908,19 +919,19 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
         <v>62</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>63</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>64</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>65</v>
-      </c>
-      <c r="E13" t="s">
-        <v>66</v>
       </c>
       <c r="F13" t="s">
         <v>11</v>
@@ -928,19 +939,19 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" t="s">
         <v>67</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>68</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>69</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>70</v>
-      </c>
-      <c r="E14" t="s">
-        <v>71</v>
       </c>
       <c r="F14" t="s">
         <v>11</v>
@@ -948,22 +959,22 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
         <v>72</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>73</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>74</v>
-      </c>
-      <c r="D15" t="s">
-        <v>73</v>
       </c>
       <c r="E15" t="s">
         <v>75</v>
       </c>
       <c r="F15" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -994,16 +1005,16 @@
         <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E17" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F17" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1074,19 +1085,859 @@
         <v>102</v>
       </c>
       <c r="C21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" t="s">
         <v>45</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" t="s">
+        <v>70</v>
+      </c>
+      <c r="F35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36" t="s">
+        <v>75</v>
+      </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" t="s">
+        <v>79</v>
+      </c>
+      <c r="E37" t="s">
+        <v>80</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" t="s">
+        <v>83</v>
+      </c>
+      <c r="D38" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" t="s">
+        <v>85</v>
+      </c>
+      <c r="F38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" t="s">
+        <v>89</v>
+      </c>
+      <c r="E39" t="s">
+        <v>90</v>
+      </c>
+      <c r="F39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" t="s">
+        <v>94</v>
+      </c>
+      <c r="E40" t="s">
+        <v>95</v>
+      </c>
+      <c r="F40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E41" t="s">
+        <v>100</v>
+      </c>
+      <c r="F41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" t="s">
         <v>103</v>
       </c>
-      <c r="E21" t="s">
+      <c r="D42" t="s">
         <v>104</v>
       </c>
-      <c r="F21" t="s">
+      <c r="E42" t="s">
+        <v>105</v>
+      </c>
+      <c r="F42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" t="s">
+        <v>23</v>
+      </c>
+      <c r="F47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48" t="s">
+        <v>29</v>
+      </c>
+      <c r="E48" t="s">
+        <v>30</v>
+      </c>
+      <c r="F48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" t="s">
+        <v>35</v>
+      </c>
+      <c r="F49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50" t="s">
+        <v>37</v>
+      </c>
+      <c r="C50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D50" t="s">
+        <v>39</v>
+      </c>
+      <c r="E50" t="s">
+        <v>40</v>
+      </c>
+      <c r="F50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" t="s">
+        <v>44</v>
+      </c>
+      <c r="E51" t="s">
+        <v>45</v>
+      </c>
+      <c r="F51" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52" t="s">
+        <v>48</v>
+      </c>
+      <c r="D52" t="s">
+        <v>49</v>
+      </c>
+      <c r="E52" t="s">
+        <v>50</v>
+      </c>
+      <c r="F52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" t="s">
+        <v>53</v>
+      </c>
+      <c r="D53" t="s">
+        <v>54</v>
+      </c>
+      <c r="E53" t="s">
+        <v>55</v>
+      </c>
+      <c r="F53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54" t="s">
+        <v>58</v>
+      </c>
+      <c r="D54" t="s">
+        <v>59</v>
+      </c>
+      <c r="E54" t="s">
+        <v>60</v>
+      </c>
+      <c r="F54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>61</v>
+      </c>
+      <c r="B55" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" t="s">
+        <v>63</v>
+      </c>
+      <c r="D55" t="s">
+        <v>64</v>
+      </c>
+      <c r="E55" t="s">
+        <v>65</v>
+      </c>
+      <c r="F55" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" t="s">
+        <v>67</v>
+      </c>
+      <c r="C56" t="s">
+        <v>68</v>
+      </c>
+      <c r="D56" t="s">
+        <v>69</v>
+      </c>
+      <c r="E56" t="s">
+        <v>70</v>
+      </c>
+      <c r="F56" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" t="s">
+        <v>72</v>
+      </c>
+      <c r="C57" t="s">
+        <v>73</v>
+      </c>
+      <c r="D57" t="s">
+        <v>74</v>
+      </c>
+      <c r="E57" t="s">
+        <v>75</v>
+      </c>
+      <c r="F57" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58" t="s">
+        <v>77</v>
+      </c>
+      <c r="C58" t="s">
+        <v>78</v>
+      </c>
+      <c r="D58" t="s">
+        <v>79</v>
+      </c>
+      <c r="E58" t="s">
+        <v>80</v>
+      </c>
+      <c r="F58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>81</v>
+      </c>
+      <c r="B59" t="s">
+        <v>82</v>
+      </c>
+      <c r="C59" t="s">
+        <v>83</v>
+      </c>
+      <c r="D59" t="s">
+        <v>84</v>
+      </c>
+      <c r="E59" t="s">
+        <v>85</v>
+      </c>
+      <c r="F59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>86</v>
+      </c>
+      <c r="B60" t="s">
+        <v>87</v>
+      </c>
+      <c r="C60" t="s">
+        <v>88</v>
+      </c>
+      <c r="D60" t="s">
+        <v>89</v>
+      </c>
+      <c r="E60" t="s">
+        <v>90</v>
+      </c>
+      <c r="F60" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>91</v>
+      </c>
+      <c r="B61" t="s">
+        <v>92</v>
+      </c>
+      <c r="C61" t="s">
+        <v>93</v>
+      </c>
+      <c r="D61" t="s">
+        <v>94</v>
+      </c>
+      <c r="E61" t="s">
+        <v>95</v>
+      </c>
+      <c r="F61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>96</v>
+      </c>
+      <c r="B62" t="s">
+        <v>97</v>
+      </c>
+      <c r="C62" t="s">
+        <v>98</v>
+      </c>
+      <c r="D62" t="s">
+        <v>99</v>
+      </c>
+      <c r="E62" t="s">
+        <v>100</v>
+      </c>
+      <c r="F62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>101</v>
+      </c>
+      <c r="B63" t="s">
+        <v>102</v>
+      </c>
+      <c r="C63" t="s">
+        <v>103</v>
+      </c>
+      <c r="D63" t="s">
+        <v>104</v>
+      </c>
+      <c r="E63" t="s">
+        <v>105</v>
+      </c>
+      <c r="F63" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
koersen bel 20 s3
Elke 10 seconden koersen ophalen van webpagina, wegschrijven naar een CSV bestand en transfereren naar S3
</commit_message>
<xml_diff>
--- a/koersen.xlsx
+++ b/koersen.xlsx
@@ -1098,7 +1098,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F126"/>
+  <dimension ref="A1:F147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
@@ -3626,6 +3626,426 @@
         <v>196</v>
       </c>
     </row>
+    <row r="127" spans="1:6">
+      <c r="A127" t="s">
+        <v>0</v>
+      </c>
+      <c r="B127" t="s">
+        <v>189</v>
+      </c>
+      <c r="C127" t="s">
+        <v>190</v>
+      </c>
+      <c r="D127" t="s">
+        <v>191</v>
+      </c>
+      <c r="E127" t="s">
+        <v>106</v>
+      </c>
+      <c r="F127" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" t="s">
+        <v>6</v>
+      </c>
+      <c r="B128" t="s">
+        <v>193</v>
+      </c>
+      <c r="C128" t="s">
+        <v>194</v>
+      </c>
+      <c r="D128" t="s">
+        <v>195</v>
+      </c>
+      <c r="E128" t="s">
+        <v>111</v>
+      </c>
+      <c r="F128" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" t="s">
+        <v>12</v>
+      </c>
+      <c r="B129" t="s">
+        <v>197</v>
+      </c>
+      <c r="C129" t="s">
+        <v>198</v>
+      </c>
+      <c r="D129" t="s">
+        <v>199</v>
+      </c>
+      <c r="E129" t="s">
+        <v>116</v>
+      </c>
+      <c r="F129" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" t="s">
+        <v>17</v>
+      </c>
+      <c r="B130" t="s">
+        <v>200</v>
+      </c>
+      <c r="C130" t="s">
+        <v>201</v>
+      </c>
+      <c r="D130" t="s">
+        <v>202</v>
+      </c>
+      <c r="E130" t="s">
+        <v>93</v>
+      </c>
+      <c r="F130" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" t="s">
+        <v>22</v>
+      </c>
+      <c r="B131" t="s">
+        <v>203</v>
+      </c>
+      <c r="C131" t="s">
+        <v>204</v>
+      </c>
+      <c r="D131" t="s">
+        <v>205</v>
+      </c>
+      <c r="E131" t="s">
+        <v>123</v>
+      </c>
+      <c r="F131" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" t="s">
+        <v>26</v>
+      </c>
+      <c r="B132" t="s">
+        <v>206</v>
+      </c>
+      <c r="C132" t="s">
+        <v>207</v>
+      </c>
+      <c r="D132" t="s">
+        <v>208</v>
+      </c>
+      <c r="E132" t="s">
+        <v>127</v>
+      </c>
+      <c r="F132" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" t="s">
+        <v>31</v>
+      </c>
+      <c r="B133" t="s">
+        <v>209</v>
+      </c>
+      <c r="C133" t="s">
+        <v>210</v>
+      </c>
+      <c r="D133" t="s">
+        <v>211</v>
+      </c>
+      <c r="E133" t="s">
+        <v>131</v>
+      </c>
+      <c r="F133" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" t="s">
+        <v>36</v>
+      </c>
+      <c r="B134" t="s">
+        <v>212</v>
+      </c>
+      <c r="C134" t="s">
+        <v>135</v>
+      </c>
+      <c r="D134" t="s">
+        <v>213</v>
+      </c>
+      <c r="E134" t="s">
+        <v>135</v>
+      </c>
+      <c r="F134" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" t="s">
+        <v>41</v>
+      </c>
+      <c r="B135" t="s">
+        <v>214</v>
+      </c>
+      <c r="C135" t="s">
+        <v>215</v>
+      </c>
+      <c r="D135" t="s">
+        <v>216</v>
+      </c>
+      <c r="E135" t="s">
+        <v>139</v>
+      </c>
+      <c r="F135" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" t="s">
+        <v>46</v>
+      </c>
+      <c r="B136" t="s">
+        <v>217</v>
+      </c>
+      <c r="C136" t="s">
+        <v>218</v>
+      </c>
+      <c r="D136" t="s">
+        <v>219</v>
+      </c>
+      <c r="E136" t="s">
+        <v>143</v>
+      </c>
+      <c r="F136" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" t="s">
+        <v>51</v>
+      </c>
+      <c r="B137" t="s">
+        <v>220</v>
+      </c>
+      <c r="C137" t="s">
+        <v>221</v>
+      </c>
+      <c r="D137" t="s">
+        <v>222</v>
+      </c>
+      <c r="E137" t="s">
+        <v>147</v>
+      </c>
+      <c r="F137" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" t="s">
+        <v>56</v>
+      </c>
+      <c r="B138" t="s">
+        <v>223</v>
+      </c>
+      <c r="C138" t="s">
+        <v>224</v>
+      </c>
+      <c r="D138" t="s">
+        <v>225</v>
+      </c>
+      <c r="E138" t="s">
+        <v>151</v>
+      </c>
+      <c r="F138" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" t="s">
+        <v>61</v>
+      </c>
+      <c r="B139" t="s">
+        <v>226</v>
+      </c>
+      <c r="C139" t="s">
+        <v>227</v>
+      </c>
+      <c r="D139" t="s">
+        <v>228</v>
+      </c>
+      <c r="E139" t="s">
+        <v>155</v>
+      </c>
+      <c r="F139" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" t="s">
+        <v>66</v>
+      </c>
+      <c r="B140" t="s">
+        <v>229</v>
+      </c>
+      <c r="C140" t="s">
+        <v>230</v>
+      </c>
+      <c r="D140" t="s">
+        <v>231</v>
+      </c>
+      <c r="E140" t="s">
+        <v>159</v>
+      </c>
+      <c r="F140" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141" t="s">
+        <v>71</v>
+      </c>
+      <c r="B141" t="s">
+        <v>232</v>
+      </c>
+      <c r="C141" t="s">
+        <v>233</v>
+      </c>
+      <c r="D141" t="s">
+        <v>234</v>
+      </c>
+      <c r="E141" t="s">
+        <v>163</v>
+      </c>
+      <c r="F141" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" t="s">
+        <v>76</v>
+      </c>
+      <c r="B142" t="s">
+        <v>235</v>
+      </c>
+      <c r="C142" t="s">
+        <v>168</v>
+      </c>
+      <c r="D142" t="s">
+        <v>236</v>
+      </c>
+      <c r="E142" t="s">
+        <v>167</v>
+      </c>
+      <c r="F142" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" t="s">
+        <v>81</v>
+      </c>
+      <c r="B143" t="s">
+        <v>170</v>
+      </c>
+      <c r="C143" t="s">
+        <v>171</v>
+      </c>
+      <c r="D143" t="s">
+        <v>237</v>
+      </c>
+      <c r="E143" t="s">
+        <v>170</v>
+      </c>
+      <c r="F143" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" t="s">
+        <v>86</v>
+      </c>
+      <c r="B144" t="s">
+        <v>238</v>
+      </c>
+      <c r="C144" t="s">
+        <v>90</v>
+      </c>
+      <c r="D144" t="s">
+        <v>239</v>
+      </c>
+      <c r="E144" t="s">
+        <v>173</v>
+      </c>
+      <c r="F144" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" t="s">
+        <v>91</v>
+      </c>
+      <c r="B145" t="s">
+        <v>240</v>
+      </c>
+      <c r="C145" t="s">
+        <v>241</v>
+      </c>
+      <c r="D145" t="s">
+        <v>242</v>
+      </c>
+      <c r="E145" t="s">
+        <v>177</v>
+      </c>
+      <c r="F145" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" t="s">
+        <v>96</v>
+      </c>
+      <c r="B146" t="s">
+        <v>243</v>
+      </c>
+      <c r="C146" t="s">
+        <v>244</v>
+      </c>
+      <c r="D146" t="s">
+        <v>245</v>
+      </c>
+      <c r="E146" t="s">
+        <v>181</v>
+      </c>
+      <c r="F146" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147" t="s">
+        <v>101</v>
+      </c>
+      <c r="B147" t="s">
+        <v>246</v>
+      </c>
+      <c r="C147" t="s">
+        <v>247</v>
+      </c>
+      <c r="D147" t="s">
+        <v>248</v>
+      </c>
+      <c r="E147" t="s">
+        <v>185</v>
+      </c>
+      <c r="F147" t="s">
+        <v>196</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>